<commit_message>
mask password +  clean up
</commit_message>
<xml_diff>
--- a/src/data/CombinedExcel.xlsx
+++ b/src/data/CombinedExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\SC2002\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887A1B7D-B0DD-485A-97FD-9D671D80A5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA59231A-8A3F-4C14-A10B-7352ECCCBD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{332BCA62-7302-4D3E-B310-571F61EE3197}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{332BCA62-7302-4D3E-B310-571F61EE3197}"/>
   </bookViews>
   <sheets>
     <sheet name="Applicants" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Managers" sheetId="2" r:id="rId3"/>
     <sheet name="ProjectListings" sheetId="4" r:id="rId4"/>
     <sheet name="Enquiries" sheetId="5" r:id="rId5"/>
-    <sheet name="FlatBookings" sheetId="6" r:id="rId6"/>
+    <sheet name="AppliedProjects" sheetId="6" r:id="rId6"/>
+    <sheet name="FlatBookings" r:id="rId10" sheetId="7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -187,43 +188,37 @@
     <t>Punggol</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>Flat Type Booked</t>
+  </si>
+  <si>
+    <t>Application Submission Date</t>
+  </si>
+  <si>
+    <t>Application Status</t>
+  </si>
+  <si>
+    <t>Units Type 1</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Units Type 2</t>
+  </si>
+  <si>
+    <t>Open Date</t>
+  </si>
+  <si>
+    <t>Close Date</t>
+  </si>
+  <si>
+    <t>Max Officer Slots</t>
   </si>
   <si>
     <t>Visibility</t>
   </si>
   <si>
     <t>true</t>
-  </si>
-  <si>
-    <t>Flat Type Booked</t>
-  </si>
-  <si>
-    <t>Application Submission Date</t>
-  </si>
-  <si>
-    <t>Application Status</t>
-  </si>
-  <si>
-    <t>Units Type 1</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Units Type 2</t>
-  </si>
-  <si>
-    <t>Open Date</t>
-  </si>
-  <si>
-    <t>Close Date</t>
-  </si>
-  <si>
-    <t>Max Officer Slots</t>
   </si>
   <si>
     <t/>
@@ -283,7 +278,7 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -624,16 +619,16 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.5703125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.08984375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.6328125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -650,7 +645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
@@ -667,7 +662,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
         <v>9</v>
       </c>
@@ -684,7 +679,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
         <v>12</v>
       </c>
@@ -701,7 +696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
         <v>14</v>
       </c>
@@ -718,7 +713,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s" s="0">
         <v>16</v>
       </c>
@@ -745,16 +740,16 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.0"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.5703125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.6328125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -771,7 +766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
         <v>22</v>
       </c>
@@ -788,7 +783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
         <v>24</v>
       </c>
@@ -805,7 +800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
         <v>26</v>
       </c>
@@ -832,16 +827,16 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.5703125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.08984375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.6328125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -858,7 +853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
         <v>18</v>
       </c>
@@ -875,7 +870,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
         <v>20</v>
       </c>
@@ -899,20 +894,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA5ED11D-0CED-4A62-BE9D-F76448168C0C}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5703125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.140625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="22.42578125"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="21.5703125"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.140625"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.42578125"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.6328125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.1796875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="22.36328125"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="21.6328125"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.08984375"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.453125"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -926,133 +921,37 @@
         <v>30</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F1" t="s" s="0">
         <v>33</v>
       </c>
       <c r="G1" t="s" s="0">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H1" t="s" s="0">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I1" t="s" s="0">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J1" t="s" s="0">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K1" t="s" s="0">
         <v>38</v>
       </c>
       <c r="L1" t="s" s="0">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="M1" t="s" s="0">
         <v>40</v>
       </c>
       <c r="N1" t="s" s="0">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>48</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="D2" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="G2" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="I2" t="n" s="3">
-        <v>45750.0</v>
-      </c>
-      <c r="J2" t="n" s="3">
-        <v>45850.0</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>61</v>
-      </c>
-      <c r="L2" t="s" s="0">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="D3" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="G3" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="I3" t="n" s="4">
-        <v>45703.0</v>
-      </c>
-      <c r="J3" t="n" s="4">
-        <v>45736.0</v>
-      </c>
-      <c r="K3" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="L3" t="s" s="0">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>46</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <v>18.0</v>
-      </c>
-      <c r="I4" t="n" s="5">
-        <v>45814.0</v>
-      </c>
-      <c r="J4" t="n" s="5">
-        <v>45844.0</v>
-      </c>
-      <c r="K4" t="s" s="0">
-        <v>61</v>
-      </c>
-      <c r="L4" t="s" s="0">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1064,30 +963,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E120475-6513-4DA8-B324-ECBFBAD860C1}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s" s="0">
         <v>28</v>
       </c>
       <c r="D1" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s" s="0">
         <v>64</v>
-      </c>
-      <c r="E1" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1096,14 +993,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA07AA4-1331-477A-93A8-BE63654CD075}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1015AB2-2D64-4477-9AB7-B5D6864FA81A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S31" sqref="S31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
@@ -1119,19 +1026,19 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s" s="0">
         <v>28</v>
       </c>
       <c r="G1" t="s" s="0">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s" s="0">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix application not showing bug
</commit_message>
<xml_diff>
--- a/src/data/CombinedExcel.xlsx
+++ b/src/data/CombinedExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\OneDrive\Desktop\NTU\SC2002 - Object Oriented Design &amp; Programing\Project\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA59231A-8A3F-4C14-A10B-7352ECCCBD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702BC9C3-1BA3-483F-B068-762A18247ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{332BCA62-7302-4D3E-B310-571F61EE3197}"/>
+    <workbookView xWindow="-24990" yWindow="3555" windowWidth="14400" windowHeight="8175" activeTab="3" xr2:uid="{332BCA62-7302-4D3E-B310-571F61EE3197}"/>
   </bookViews>
   <sheets>
     <sheet name="Applicants" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,11 @@
     <sheet name="Managers" sheetId="2" r:id="rId3"/>
     <sheet name="ProjectListings" sheetId="4" r:id="rId4"/>
     <sheet name="Enquiries" sheetId="5" r:id="rId5"/>
-    <sheet name="AppliedProjects" sheetId="6" r:id="rId6"/>
-    <sheet name="FlatBookings" r:id="rId10" sheetId="7"/>
+    <sheet name="FlatBookings" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -137,33 +136,12 @@
     <t>Type 1</t>
   </si>
   <si>
-    <t>Number of units for Type 1</t>
-  </si>
-  <si>
-    <t>Selling price for Type 1</t>
-  </si>
-  <si>
     <t>Type 2</t>
   </si>
   <si>
-    <t>Number of units for Type 2</t>
-  </si>
-  <si>
-    <t>Selling price for Type 2</t>
-  </si>
-  <si>
-    <t>Application opening date</t>
-  </si>
-  <si>
-    <t>Application closing date</t>
-  </si>
-  <si>
     <t>Manager</t>
   </si>
   <si>
-    <t>Officer Slot</t>
-  </si>
-  <si>
     <t>Officer</t>
   </si>
   <si>
@@ -179,9 +157,6 @@
     <t>3-Room</t>
   </si>
   <si>
-    <t>Daniel,Emily</t>
-  </si>
-  <si>
     <t>Twin Waterfall</t>
   </si>
   <si>
@@ -218,34 +193,67 @@
     <t>Visibility</t>
   </si>
   <si>
+    <t>Enquiry ID</t>
+  </si>
+  <si>
+    <t>Sender NRIC</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Reply</t>
+  </si>
+  <si>
+    <t>Replied By</t>
+  </si>
+  <si>
     <t>true</t>
   </si>
   <si>
+    <t>hi</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Enquiry ID</t>
-  </si>
-  <si>
-    <t>Sender NRIC</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
-    <t>Reply</t>
-  </si>
-  <si>
-    <t>Replied By</t>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>SUCCESSFUL</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>S7894523E</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>PENDING</t>
+  </si>
+  <si>
+    <t>UNSUCCESSFUL</t>
+  </si>
+  <si>
+    <t>idk</t>
+  </si>
+  <si>
+    <t>asafsadf</t>
+  </si>
+  <si>
+    <t>tekong</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d/M/yyyy"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -275,13 +283,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,117 +620,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4174EED-D054-4CF2-9DCF-AF869BD95E43}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.08984375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.6328125"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>35</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>40</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4">
         <v>37</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="0">
+      <c r="C5">
         <v>30</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="0">
+      <c r="C6">
         <v>25</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -745,75 +766,75 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.0"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.6328125"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>36</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>28</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4">
         <v>29</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -832,58 +853,58 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.08984375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.6328125"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>36</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>26</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -894,64 +915,357 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA5ED11D-0CED-4A62-BE9D-F76448168C0C}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.6328125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.1796875"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="22.36328125"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="21.6328125"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.08984375"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.453125"/>
+    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="E1" t="s" s="0">
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>450000</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>650000</v>
+      </c>
+      <c r="I2" s="1">
+        <v>46068</v>
+      </c>
+      <c r="J2" s="1">
+        <v>46101</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2">
+        <v>7</v>
+      </c>
+      <c r="N2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>450000</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>650000</v>
+      </c>
+      <c r="I3" s="1">
+        <v>46069</v>
+      </c>
+      <c r="J3" s="1">
+        <v>46101</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3">
+        <v>8</v>
+      </c>
+      <c r="N3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>450000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4">
+        <v>23</v>
+      </c>
+      <c r="H4">
+        <v>650000</v>
+      </c>
+      <c r="I4" s="1">
+        <v>46066</v>
+      </c>
+      <c r="J4" s="1">
+        <v>46101</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="N4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>450000</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5">
+        <v>32</v>
+      </c>
+      <c r="H5">
+        <v>650000</v>
+      </c>
+      <c r="I5" s="1">
+        <v>46067</v>
+      </c>
+      <c r="J5" s="1">
+        <v>46101</v>
+      </c>
+      <c r="K5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5">
+        <v>6</v>
+      </c>
+      <c r="N5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>450000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6">
         <v>52</v>
       </c>
-      <c r="F1" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="G1" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="H1" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="I1" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="J1" t="s" s="0">
+      <c r="H6">
+        <v>650000</v>
+      </c>
+      <c r="I6" s="1">
+        <v>45700</v>
+      </c>
+      <c r="J6" s="1">
+        <v>45736</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" t="s">
         <v>55</v>
       </c>
-      <c r="K1" t="s" s="0">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>350000</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>450000</v>
+      </c>
+      <c r="I7" s="1">
+        <v>45740</v>
+      </c>
+      <c r="J7" s="1">
+        <v>46101</v>
+      </c>
+      <c r="K7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>38</v>
       </c>
-      <c r="L1" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="M1" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="N1" t="s" s="0">
-        <v>57</v>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>450000</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>650000</v>
+      </c>
+      <c r="I8" s="1">
+        <v>45700</v>
+      </c>
+      <c r="J8" s="1">
+        <v>46101</v>
+      </c>
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="N8" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -961,30 +1275,72 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E120475-6513-4DA8-B324-ECBFBAD860C1}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s" s="0">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s" s="0">
-        <v>62</v>
-      </c>
-      <c r="E1" t="s" s="0">
-        <v>63</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>64</v>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -993,52 +1349,208 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1015AB2-2D64-4477-9AB7-B5D6864FA81A}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="1">
+        <v>45715</v>
+      </c>
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="1">
+        <v>45771</v>
+      </c>
+      <c r="H3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="1">
+        <v>45775</v>
+      </c>
+      <c r="H4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="1">
+        <v>45772</v>
+      </c>
+      <c r="H5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="1">
+        <v>45770</v>
+      </c>
+      <c r="H6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="1">
+        <v>45773</v>
+      </c>
+      <c r="H7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s" s="0">
-        <v>48</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="H1" t="s" s="0">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>